<commit_message>
Updated Pattern for Master.xlsx
</commit_message>
<xml_diff>
--- a/master.xlsx
+++ b/master.xlsx
@@ -1,31 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Mendine\Test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aritra Palit\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB7B35C1-5E0B-4ACD-81E2-A144829EBF13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B07D37-783A-4131-9D66-79A805820948}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Usernames" sheetId="1" r:id="rId1"/>
+    <sheet name="Medicines" sheetId="2" r:id="rId2"/>
+    <sheet name="Customer" sheetId="3" r:id="rId3"/>
+    <sheet name="Bills" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>Username</t>
   </si>
@@ -33,7 +31,58 @@
     <t>Password</t>
   </si>
   <si>
-    <t>aritra</t>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Emp_ID</t>
+  </si>
+  <si>
+    <t>MedicineID</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>dateAdded</t>
+  </si>
+  <si>
+    <t>lastUpdated</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Timestamp</t>
+  </si>
+  <si>
+    <t>User ID</t>
+  </si>
+  <si>
+    <t>User Name</t>
+  </si>
+  <si>
+    <t>Customer Phone</t>
+  </si>
+  <si>
+    <t>Customer Name</t>
+  </si>
+  <si>
+    <t>Customer Address</t>
+  </si>
+  <si>
+    <t>Total Amount</t>
+  </si>
+  <si>
+    <t>Products</t>
+  </si>
+  <si>
+    <t>Prices</t>
   </si>
 </sst>
 </file>
@@ -69,8 +118,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -351,29 +403,156 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
-        <v>1234</v>
+      <c r="D1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:I25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S19" sqref="S19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="8:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H25" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>